<commit_message>
Aggiornato da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/delivery.xlsx
+++ b/delivery.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26480" uniqueCount="5587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27680" uniqueCount="5818">
   <si>
     <t>Codice</t>
   </si>
@@ -16778,6 +16778,699 @@
   </si>
   <si>
     <t>B37200319</t>
+  </si>
+  <si>
+    <t>ADSL1004496226</t>
+  </si>
+  <si>
+    <t>90880470</t>
+  </si>
+  <si>
+    <t>08/08/2025</t>
+  </si>
+  <si>
+    <t>CONTRADA GRANELLI SNC</t>
+  </si>
+  <si>
+    <t>08/08/2025 15:00</t>
+  </si>
+  <si>
+    <t>DTU0065829930</t>
+  </si>
+  <si>
+    <t>93114759325</t>
+  </si>
+  <si>
+    <t>E70090880470</t>
+  </si>
+  <si>
+    <t>30/06/2025 11:48</t>
+  </si>
+  <si>
+    <t>B36201365</t>
+  </si>
+  <si>
+    <t>ADSL1004596246</t>
+  </si>
+  <si>
+    <t>91545436</t>
+  </si>
+  <si>
+    <t>VIA FLORIDIANI DI HARTFORD 43</t>
+  </si>
+  <si>
+    <t>08/08/2025 10:30</t>
+  </si>
+  <si>
+    <t>DTU0066211775</t>
+  </si>
+  <si>
+    <t>G600069366</t>
+  </si>
+  <si>
+    <t>E70091545436</t>
+  </si>
+  <si>
+    <t>22/07/2025 12:46</t>
+  </si>
+  <si>
+    <t>B36804632</t>
+  </si>
+  <si>
+    <t>ADSL1004601422</t>
+  </si>
+  <si>
+    <t>91576395</t>
+  </si>
+  <si>
+    <t>VIA SANTA ALESSANDRA 200</t>
+  </si>
+  <si>
+    <t>DTU0066245196</t>
+  </si>
+  <si>
+    <t>93114726312</t>
+  </si>
+  <si>
+    <t>E70091576395</t>
+  </si>
+  <si>
+    <t>23/07/2025 11:52</t>
+  </si>
+  <si>
+    <t>B36832445</t>
+  </si>
+  <si>
+    <t>ADSL1004604327</t>
+  </si>
+  <si>
+    <t>91594942</t>
+  </si>
+  <si>
+    <t>VICO MANFREDONIA 62</t>
+  </si>
+  <si>
+    <t>08/08/2025 08:30</t>
+  </si>
+  <si>
+    <t>DTU0066206799</t>
+  </si>
+  <si>
+    <t>93114731603</t>
+  </si>
+  <si>
+    <t>E70091594942</t>
+  </si>
+  <si>
+    <t>23/07/2025 19:58</t>
+  </si>
+  <si>
+    <t>B36846450</t>
+  </si>
+  <si>
+    <t>ADSL1004638859</t>
+  </si>
+  <si>
+    <t>91818922</t>
+  </si>
+  <si>
+    <t>09/08/2025</t>
+  </si>
+  <si>
+    <t>VIA BUON PASTORE 9</t>
+  </si>
+  <si>
+    <t>DTU0066424201</t>
+  </si>
+  <si>
+    <t>93114720984</t>
+  </si>
+  <si>
+    <t>E70091818922</t>
+  </si>
+  <si>
+    <t>31/07/2025 21:08</t>
+  </si>
+  <si>
+    <t>B37054854</t>
+  </si>
+  <si>
+    <t>ADSL1004638901</t>
+  </si>
+  <si>
+    <t>91819072</t>
+  </si>
+  <si>
+    <t>VIA DELLE ORTENSIE - CASSIBILE 23</t>
+  </si>
+  <si>
+    <t>DTU0066417860</t>
+  </si>
+  <si>
+    <t>0931861753</t>
+  </si>
+  <si>
+    <t>E70091819072</t>
+  </si>
+  <si>
+    <t>31/07/2025 21:24</t>
+  </si>
+  <si>
+    <t>B37055037</t>
+  </si>
+  <si>
+    <t>ADSL1004640147</t>
+  </si>
+  <si>
+    <t>91828827</t>
+  </si>
+  <si>
+    <t>V. SERGIO SALLICANO 7</t>
+  </si>
+  <si>
+    <t>DTU0066432422</t>
+  </si>
+  <si>
+    <t>0931892130</t>
+  </si>
+  <si>
+    <t>E70091828827</t>
+  </si>
+  <si>
+    <t>01/08/2025 11:30</t>
+  </si>
+  <si>
+    <t>B37067392</t>
+  </si>
+  <si>
+    <t>ADSL1004644155</t>
+  </si>
+  <si>
+    <t>91852385</t>
+  </si>
+  <si>
+    <t>VIA SAN MARTINO 21</t>
+  </si>
+  <si>
+    <t>DTU0066447965</t>
+  </si>
+  <si>
+    <t>93114724406</t>
+  </si>
+  <si>
+    <t>E70091852385</t>
+  </si>
+  <si>
+    <t>02/08/2025 08:22</t>
+  </si>
+  <si>
+    <t>B37089921</t>
+  </si>
+  <si>
+    <t>ADSL1004644177</t>
+  </si>
+  <si>
+    <t>91852526</t>
+  </si>
+  <si>
+    <t>DTU0066444847</t>
+  </si>
+  <si>
+    <t>93114759494</t>
+  </si>
+  <si>
+    <t>E70091852526</t>
+  </si>
+  <si>
+    <t>B37090053</t>
+  </si>
+  <si>
+    <t>ADSL1004649119</t>
+  </si>
+  <si>
+    <t>91882851</t>
+  </si>
+  <si>
+    <t>E70091882851</t>
+  </si>
+  <si>
+    <t>04/08/2025 11:34</t>
+  </si>
+  <si>
+    <t>B37123909</t>
+  </si>
+  <si>
+    <t>ADSL1004651015</t>
+  </si>
+  <si>
+    <t>91896339</t>
+  </si>
+  <si>
+    <t>VIALE VITTORIO VENETO 168</t>
+  </si>
+  <si>
+    <t>08/08/2025 13:00</t>
+  </si>
+  <si>
+    <t>DTU0066471503</t>
+  </si>
+  <si>
+    <t>0931314256</t>
+  </si>
+  <si>
+    <t>E70091896339</t>
+  </si>
+  <si>
+    <t>04/08/2025 16:02</t>
+  </si>
+  <si>
+    <t>B37133668</t>
+  </si>
+  <si>
+    <t>ADSL1004651849</t>
+  </si>
+  <si>
+    <t>91901631</t>
+  </si>
+  <si>
+    <t>VIA ROCCO CHINNICI 35</t>
+  </si>
+  <si>
+    <t>DTU0066473590</t>
+  </si>
+  <si>
+    <t>0931861023</t>
+  </si>
+  <si>
+    <t>E70091901631</t>
+  </si>
+  <si>
+    <t>04/08/2025 18:24</t>
+  </si>
+  <si>
+    <t>B37137619</t>
+  </si>
+  <si>
+    <t>ADSL1004653710</t>
+  </si>
+  <si>
+    <t>91913426</t>
+  </si>
+  <si>
+    <t>VIA GORIZIA 29</t>
+  </si>
+  <si>
+    <t>DTU0066468947</t>
+  </si>
+  <si>
+    <t>0931861779</t>
+  </si>
+  <si>
+    <t>E70091913426</t>
+  </si>
+  <si>
+    <t>05/08/2025 10:46</t>
+  </si>
+  <si>
+    <t>B37150991</t>
+  </si>
+  <si>
+    <t>ADSL1004655319</t>
+  </si>
+  <si>
+    <t>91925218</t>
+  </si>
+  <si>
+    <t>VIA OLINTO MARINELLI 60</t>
+  </si>
+  <si>
+    <t>DTU0066392758</t>
+  </si>
+  <si>
+    <t>0931861788</t>
+  </si>
+  <si>
+    <t>E70091925218</t>
+  </si>
+  <si>
+    <t>05/08/2025 14:26</t>
+  </si>
+  <si>
+    <t>B37159844</t>
+  </si>
+  <si>
+    <t>ADSL1004657179</t>
+  </si>
+  <si>
+    <t>91940618</t>
+  </si>
+  <si>
+    <t>STRADA MONASTERI 21</t>
+  </si>
+  <si>
+    <t>DTU0066488291</t>
+  </si>
+  <si>
+    <t>0931861351</t>
+  </si>
+  <si>
+    <t>E70091940618</t>
+  </si>
+  <si>
+    <t>05/08/2025 18:58</t>
+  </si>
+  <si>
+    <t>B37171790</t>
+  </si>
+  <si>
+    <t>ADSL1004658110</t>
+  </si>
+  <si>
+    <t>91944912</t>
+  </si>
+  <si>
+    <t>VIA PITAGORA 9</t>
+  </si>
+  <si>
+    <t>DTU0066490344</t>
+  </si>
+  <si>
+    <t>93114759507</t>
+  </si>
+  <si>
+    <t>E70091944912</t>
+  </si>
+  <si>
+    <t>06/08/2025 00:42</t>
+  </si>
+  <si>
+    <t>B37176245</t>
+  </si>
+  <si>
+    <t>ADSL1004658476</t>
+  </si>
+  <si>
+    <t>91948219</t>
+  </si>
+  <si>
+    <t>VIA FRATELLI ROSSELLI 16</t>
+  </si>
+  <si>
+    <t>DTU0066470868</t>
+  </si>
+  <si>
+    <t>93114757711</t>
+  </si>
+  <si>
+    <t>E70091948219</t>
+  </si>
+  <si>
+    <t>06/08/2025 09:26</t>
+  </si>
+  <si>
+    <t>B37183066</t>
+  </si>
+  <si>
+    <t>ADSL1004658565</t>
+  </si>
+  <si>
+    <t>91949213</t>
+  </si>
+  <si>
+    <t>VIA UGO FOSCOLO 2</t>
+  </si>
+  <si>
+    <t>DTU0066231131</t>
+  </si>
+  <si>
+    <t>0931861633</t>
+  </si>
+  <si>
+    <t>E70091949213</t>
+  </si>
+  <si>
+    <t>06/08/2025 09:46</t>
+  </si>
+  <si>
+    <t>B37183836</t>
+  </si>
+  <si>
+    <t>ADSL1004661531</t>
+  </si>
+  <si>
+    <t>91968308</t>
+  </si>
+  <si>
+    <t>VICO MOLISE 25</t>
+  </si>
+  <si>
+    <t>DTU0064870957</t>
+  </si>
+  <si>
+    <t>G600060765</t>
+  </si>
+  <si>
+    <t>E70091968308</t>
+  </si>
+  <si>
+    <t>06/08/2025 16:24</t>
+  </si>
+  <si>
+    <t>B37198489</t>
+  </si>
+  <si>
+    <t>ADSL1004662186</t>
+  </si>
+  <si>
+    <t>91971616</t>
+  </si>
+  <si>
+    <t>VIA GIOVANNI GIOLITTI 13</t>
+  </si>
+  <si>
+    <t>08/08/2025 17:00</t>
+  </si>
+  <si>
+    <t>DTU0066435088</t>
+  </si>
+  <si>
+    <t>93114737186</t>
+  </si>
+  <si>
+    <t>E70091971616</t>
+  </si>
+  <si>
+    <t>06/08/2025 17:58</t>
+  </si>
+  <si>
+    <t>B37200990</t>
+  </si>
+  <si>
+    <t>ADSL1004662196</t>
+  </si>
+  <si>
+    <t>91971643</t>
+  </si>
+  <si>
+    <t>VIA DANTE ALIGHIERI 157</t>
+  </si>
+  <si>
+    <t>DTU0066434990</t>
+  </si>
+  <si>
+    <t>93114759348</t>
+  </si>
+  <si>
+    <t>E70091971643</t>
+  </si>
+  <si>
+    <t>B37200959</t>
+  </si>
+  <si>
+    <t>ADSL1004662616</t>
+  </si>
+  <si>
+    <t>91974133</t>
+  </si>
+  <si>
+    <t>VIA ALESSANDRO MANZONI 162</t>
+  </si>
+  <si>
+    <t>DTU0066383168</t>
+  </si>
+  <si>
+    <t>93114732508</t>
+  </si>
+  <si>
+    <t>E70091974133</t>
+  </si>
+  <si>
+    <t>06/08/2025 19:54</t>
+  </si>
+  <si>
+    <t>B37202916</t>
+  </si>
+  <si>
+    <t>ADSL1004663824</t>
+  </si>
+  <si>
+    <t>91981788</t>
+  </si>
+  <si>
+    <t>DTU0066507604</t>
+  </si>
+  <si>
+    <t>0931861133</t>
+  </si>
+  <si>
+    <t>E70091981788</t>
+  </si>
+  <si>
+    <t>07/08/2025 10:20</t>
+  </si>
+  <si>
+    <t>B37215093</t>
+  </si>
+  <si>
+    <t>ADSL1004664757</t>
+  </si>
+  <si>
+    <t>91989708</t>
+  </si>
+  <si>
+    <t>VIA MIDDLETOWN CONNECTICUT 4</t>
+  </si>
+  <si>
+    <t>DTU0066188568</t>
+  </si>
+  <si>
+    <t>0931861991</t>
+  </si>
+  <si>
+    <t>E70091989708</t>
+  </si>
+  <si>
+    <t>07/08/2025 12:58</t>
+  </si>
+  <si>
+    <t>B37222502</t>
+  </si>
+  <si>
+    <t>ADSL1004665607</t>
+  </si>
+  <si>
+    <t>91995534</t>
+  </si>
+  <si>
+    <t>VIA G.CONSIGLIO 15</t>
+  </si>
+  <si>
+    <t>09/08/2025 08:30</t>
+  </si>
+  <si>
+    <t>DTU0066503104</t>
+  </si>
+  <si>
+    <t>93114732457</t>
+  </si>
+  <si>
+    <t>E70091995534</t>
+  </si>
+  <si>
+    <t>07/08/2025 14:58</t>
+  </si>
+  <si>
+    <t>B37226774</t>
+  </si>
+  <si>
+    <t>ADSL1004665642</t>
+  </si>
+  <si>
+    <t>91995775</t>
+  </si>
+  <si>
+    <t>VIA TINTORETTO 10</t>
+  </si>
+  <si>
+    <t>DTU0066510487</t>
+  </si>
+  <si>
+    <t>0931861102</t>
+  </si>
+  <si>
+    <t>E70091995775</t>
+  </si>
+  <si>
+    <t>07/08/2025 15:04</t>
+  </si>
+  <si>
+    <t>B37226913</t>
+  </si>
+  <si>
+    <t>ADSL1004665648</t>
+  </si>
+  <si>
+    <t>91995781</t>
+  </si>
+  <si>
+    <t>VIA TENENTE SIPIONE 52</t>
+  </si>
+  <si>
+    <t>DTU0066500280</t>
+  </si>
+  <si>
+    <t>0931861794</t>
+  </si>
+  <si>
+    <t>E70091995781</t>
+  </si>
+  <si>
+    <t>B37226911</t>
+  </si>
+  <si>
+    <t>ADSL1004665674</t>
+  </si>
+  <si>
+    <t>91995861</t>
+  </si>
+  <si>
+    <t>VIA GIOVANNI PASCOLI 12</t>
+  </si>
+  <si>
+    <t>DTU0066166667</t>
+  </si>
+  <si>
+    <t>93114743815</t>
+  </si>
+  <si>
+    <t>E70091995861</t>
+  </si>
+  <si>
+    <t>B37226947</t>
+  </si>
+  <si>
+    <t>ADSL1004667851</t>
+  </si>
+  <si>
+    <t>92008667</t>
+  </si>
+  <si>
+    <t>VIA D'AGATA MICALE 73</t>
+  </si>
+  <si>
+    <t>DTU0066532798</t>
+  </si>
+  <si>
+    <t>93114757375</t>
+  </si>
+  <si>
+    <t>E70092008667</t>
+  </si>
+  <si>
+    <t>07/08/2025 23:00</t>
+  </si>
+  <si>
+    <t>B37237662</t>
   </si>
 </sst>
 </file>
@@ -17107,10 +17800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN662"/>
+  <dimension ref="A1:AN692"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="A647" workbookViewId="0">
+      <selection activeCell="B665" sqref="B665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -97885,6 +98578,3666 @@
         <v>5586</v>
       </c>
     </row>
+    <row r="663" spans="1:40">
+      <c r="A663" s="1" t="s">
+        <v>5587</v>
+      </c>
+      <c r="B663" s="1" t="s">
+        <v>5588</v>
+      </c>
+      <c r="C663" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D663" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E663" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K663" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L663" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="M663" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="N663" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O663" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P663" s="1" t="s">
+        <v>5590</v>
+      </c>
+      <c r="Q663" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R663" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S663" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T663" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U663" s="1" t="s">
+        <v>5592</v>
+      </c>
+      <c r="V663" s="1" t="s">
+        <v>5593</v>
+      </c>
+      <c r="W663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X663" s="1" t="s">
+        <v>5594</v>
+      </c>
+      <c r="Y663" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z663" s="1" t="s">
+        <v>5595</v>
+      </c>
+      <c r="AA663" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB663" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC663" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD663" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE663" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF663" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG663" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI663" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK663" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM663" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN663" s="1" t="s">
+        <v>5596</v>
+      </c>
+    </row>
+    <row r="664" spans="1:40">
+      <c r="A664" s="1" t="s">
+        <v>5597</v>
+      </c>
+      <c r="B664" s="1" t="s">
+        <v>5598</v>
+      </c>
+      <c r="C664" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D664" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E664" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K664" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L664" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M664" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N664" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O664" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="P664" s="1" t="s">
+        <v>5599</v>
+      </c>
+      <c r="Q664" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R664" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S664" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T664" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U664" s="1" t="s">
+        <v>5601</v>
+      </c>
+      <c r="V664" s="1" t="s">
+        <v>5602</v>
+      </c>
+      <c r="W664" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X664" s="1" t="s">
+        <v>5603</v>
+      </c>
+      <c r="Y664" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z664" s="1" t="s">
+        <v>5604</v>
+      </c>
+      <c r="AA664" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB664" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC664" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD664" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE664" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="AF664" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG664" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="AH664" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="AI664" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK664" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM664" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN664" s="1" t="s">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="665" spans="1:40">
+      <c r="A665" s="1" t="s">
+        <v>5606</v>
+      </c>
+      <c r="B665" s="1" t="s">
+        <v>5607</v>
+      </c>
+      <c r="C665" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D665" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E665" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K665" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L665" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M665" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N665" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O665" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P665" s="1" t="s">
+        <v>5608</v>
+      </c>
+      <c r="Q665" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R665" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S665" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T665" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U665" s="1" t="s">
+        <v>5609</v>
+      </c>
+      <c r="V665" s="1" t="s">
+        <v>5610</v>
+      </c>
+      <c r="W665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X665" s="1" t="s">
+        <v>5611</v>
+      </c>
+      <c r="Y665" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z665" s="1" t="s">
+        <v>5612</v>
+      </c>
+      <c r="AA665" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB665" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC665" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD665" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE665" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF665" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG665" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI665" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK665" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL665" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM665" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN665" s="1" t="s">
+        <v>5613</v>
+      </c>
+    </row>
+    <row r="666" spans="1:40">
+      <c r="A666" s="1" t="s">
+        <v>5614</v>
+      </c>
+      <c r="B666" s="1" t="s">
+        <v>5615</v>
+      </c>
+      <c r="C666" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D666" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E666" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F666" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G666" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H666" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I666" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J666" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K666" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L666" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="M666" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N666" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O666" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P666" s="1" t="s">
+        <v>5616</v>
+      </c>
+      <c r="Q666" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="R666" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S666" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T666" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U666" s="1" t="s">
+        <v>5618</v>
+      </c>
+      <c r="V666" s="1" t="s">
+        <v>5619</v>
+      </c>
+      <c r="W666" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X666" s="1" t="s">
+        <v>5620</v>
+      </c>
+      <c r="Y666" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z666" s="1" t="s">
+        <v>5621</v>
+      </c>
+      <c r="AA666" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AB666" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AC666" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD666" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE666" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF666" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG666" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH666" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI666" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ666" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK666" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL666" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM666" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN666" s="1" t="s">
+        <v>5622</v>
+      </c>
+    </row>
+    <row r="667" spans="1:40">
+      <c r="A667" s="1" t="s">
+        <v>5623</v>
+      </c>
+      <c r="B667" s="1" t="s">
+        <v>5624</v>
+      </c>
+      <c r="C667" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="D667" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E667" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F667" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G667" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H667" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I667" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J667" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K667" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L667" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M667" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N667" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O667" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P667" s="1" t="s">
+        <v>5626</v>
+      </c>
+      <c r="Q667" s="1" t="s">
+        <v>5231</v>
+      </c>
+      <c r="R667" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S667" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T667" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U667" s="1" t="s">
+        <v>5627</v>
+      </c>
+      <c r="V667" s="1" t="s">
+        <v>5628</v>
+      </c>
+      <c r="W667" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X667" s="1" t="s">
+        <v>5629</v>
+      </c>
+      <c r="Y667" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z667" s="1" t="s">
+        <v>5630</v>
+      </c>
+      <c r="AA667" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB667" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC667" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD667" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE667" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF667" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG667" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH667" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI667" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ667" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK667" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL667" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM667" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN667" s="1" t="s">
+        <v>5631</v>
+      </c>
+    </row>
+    <row r="668" spans="1:40">
+      <c r="A668" s="1" t="s">
+        <v>5632</v>
+      </c>
+      <c r="B668" s="1" t="s">
+        <v>5633</v>
+      </c>
+      <c r="C668" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D668" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E668" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F668" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G668" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H668" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="I668" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="J668" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K668" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L668" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M668" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N668" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O668" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P668" s="1" t="s">
+        <v>5634</v>
+      </c>
+      <c r="Q668" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R668" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S668" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T668" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U668" s="1" t="s">
+        <v>5635</v>
+      </c>
+      <c r="V668" s="1" t="s">
+        <v>5636</v>
+      </c>
+      <c r="W668" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X668" s="1" t="s">
+        <v>5637</v>
+      </c>
+      <c r="Y668" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z668" s="1" t="s">
+        <v>5638</v>
+      </c>
+      <c r="AA668" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB668" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC668" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD668" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE668" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF668" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG668" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH668" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI668" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ668" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK668" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL668" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM668" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN668" s="1" t="s">
+        <v>5639</v>
+      </c>
+    </row>
+    <row r="669" spans="1:40">
+      <c r="A669" s="1" t="s">
+        <v>5640</v>
+      </c>
+      <c r="B669" s="1" t="s">
+        <v>5641</v>
+      </c>
+      <c r="C669" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D669" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E669" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F669" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G669" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H669" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I669" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J669" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="K669" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="L669" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M669" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N669" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O669" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P669" s="1" t="s">
+        <v>5642</v>
+      </c>
+      <c r="Q669" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="R669" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S669" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T669" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U669" s="1" t="s">
+        <v>5643</v>
+      </c>
+      <c r="V669" s="1" t="s">
+        <v>5644</v>
+      </c>
+      <c r="W669" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X669" s="1" t="s">
+        <v>5645</v>
+      </c>
+      <c r="Y669" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z669" s="1" t="s">
+        <v>5646</v>
+      </c>
+      <c r="AA669" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB669" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC669" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD669" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE669" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF669" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG669" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH669" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI669" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ669" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK669" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL669" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="AM669" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN669" s="1" t="s">
+        <v>5647</v>
+      </c>
+    </row>
+    <row r="670" spans="1:40">
+      <c r="A670" s="1" t="s">
+        <v>5227</v>
+      </c>
+      <c r="B670" s="1" t="s">
+        <v>5228</v>
+      </c>
+      <c r="C670" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="D670" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E670" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F670" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="G670" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H670" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I670" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J670" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K670" s="1" t="s">
+        <v>5229</v>
+      </c>
+      <c r="L670" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="M670" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N670" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O670" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P670" s="1" t="s">
+        <v>5230</v>
+      </c>
+      <c r="Q670" s="1" t="s">
+        <v>5231</v>
+      </c>
+      <c r="R670" s="1" t="s">
+        <v>5250</v>
+      </c>
+      <c r="S670" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T670" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="U670" s="1" t="s">
+        <v>5233</v>
+      </c>
+      <c r="V670" s="1" t="s">
+        <v>5234</v>
+      </c>
+      <c r="W670" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X670" s="1" t="s">
+        <v>5235</v>
+      </c>
+      <c r="Y670" s="1" t="s">
+        <v>5236</v>
+      </c>
+      <c r="Z670" s="1" t="s">
+        <v>5237</v>
+      </c>
+      <c r="AA670" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB670" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC670" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD670" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE670" s="1" t="s">
+        <v>5238</v>
+      </c>
+      <c r="AF670" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG670" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH670" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI670" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ670" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK670" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL670" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM670" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN670" s="1" t="s">
+        <v>5239</v>
+      </c>
+    </row>
+    <row r="671" spans="1:40">
+      <c r="A671" s="1" t="s">
+        <v>5648</v>
+      </c>
+      <c r="B671" s="1" t="s">
+        <v>5649</v>
+      </c>
+      <c r="C671" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D671" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E671" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F671" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G671" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H671" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I671" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J671" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K671" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L671" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M671" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N671" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O671" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P671" s="1" t="s">
+        <v>5650</v>
+      </c>
+      <c r="Q671" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R671" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S671" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T671" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U671" s="1" t="s">
+        <v>5651</v>
+      </c>
+      <c r="V671" s="1" t="s">
+        <v>5652</v>
+      </c>
+      <c r="W671" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X671" s="1" t="s">
+        <v>5653</v>
+      </c>
+      <c r="Y671" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z671" s="1" t="s">
+        <v>5654</v>
+      </c>
+      <c r="AA671" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB671" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC671" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD671" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE671" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF671" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG671" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH671" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI671" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ671" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK671" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL671" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM671" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN671" s="1" t="s">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="672" spans="1:40">
+      <c r="A672" s="1" t="s">
+        <v>5656</v>
+      </c>
+      <c r="B672" s="1" t="s">
+        <v>5657</v>
+      </c>
+      <c r="C672" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D672" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E672" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F672" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G672" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H672" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I672" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J672" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K672" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L672" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M672" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N672" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O672" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P672" s="1" t="s">
+        <v>2164</v>
+      </c>
+      <c r="Q672" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="R672" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S672" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T672" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U672" s="1" t="s">
+        <v>5658</v>
+      </c>
+      <c r="V672" s="1" t="s">
+        <v>5659</v>
+      </c>
+      <c r="W672" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X672" s="1" t="s">
+        <v>5660</v>
+      </c>
+      <c r="Y672" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z672" s="1" t="s">
+        <v>3194</v>
+      </c>
+      <c r="AA672" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB672" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC672" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD672" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE672" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF672" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG672" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH672" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI672" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ672" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK672" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL672" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM672" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN672" s="1" t="s">
+        <v>5661</v>
+      </c>
+    </row>
+    <row r="673" spans="1:40">
+      <c r="A673" s="1" t="s">
+        <v>5662</v>
+      </c>
+      <c r="B673" s="1" t="s">
+        <v>5663</v>
+      </c>
+      <c r="C673" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D673" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E673" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F673" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G673" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H673" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I673" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J673" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K673" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L673" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M673" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N673" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O673" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P673" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="Q673" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R673" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S673" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T673" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U673" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="V673" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="W673" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X673" s="1" t="s">
+        <v>5664</v>
+      </c>
+      <c r="Y673" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z673" s="1" t="s">
+        <v>5665</v>
+      </c>
+      <c r="AA673" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB673" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC673" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD673" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE673" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF673" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG673" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH673" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI673" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ673" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK673" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL673" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM673" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN673" s="1" t="s">
+        <v>5666</v>
+      </c>
+    </row>
+    <row r="674" spans="1:40">
+      <c r="A674" s="1" t="s">
+        <v>5667</v>
+      </c>
+      <c r="B674" s="1" t="s">
+        <v>5668</v>
+      </c>
+      <c r="C674" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D674" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E674" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K674" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L674" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M674" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N674" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O674" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P674" s="1" t="s">
+        <v>5669</v>
+      </c>
+      <c r="Q674" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="R674" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S674" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T674" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U674" s="1" t="s">
+        <v>5671</v>
+      </c>
+      <c r="V674" s="1" t="s">
+        <v>5672</v>
+      </c>
+      <c r="W674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X674" s="1" t="s">
+        <v>5673</v>
+      </c>
+      <c r="Y674" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z674" s="1" t="s">
+        <v>5674</v>
+      </c>
+      <c r="AA674" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB674" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC674" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD674" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE674" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF674" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG674" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH674" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI674" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK674" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL674" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM674" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN674" s="1" t="s">
+        <v>5675</v>
+      </c>
+    </row>
+    <row r="675" spans="1:40">
+      <c r="A675" s="1" t="s">
+        <v>5676</v>
+      </c>
+      <c r="B675" s="1" t="s">
+        <v>5677</v>
+      </c>
+      <c r="C675" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D675" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E675" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F675" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G675" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H675" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I675" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J675" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K675" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L675" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M675" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N675" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O675" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P675" s="1" t="s">
+        <v>5678</v>
+      </c>
+      <c r="Q675" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R675" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S675" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T675" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U675" s="1" t="s">
+        <v>5679</v>
+      </c>
+      <c r="V675" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="W675" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X675" s="1" t="s">
+        <v>5681</v>
+      </c>
+      <c r="Y675" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z675" s="1" t="s">
+        <v>5682</v>
+      </c>
+      <c r="AA675" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB675" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC675" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD675" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE675" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF675" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG675" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH675" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI675" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ675" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK675" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL675" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM675" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN675" s="1" t="s">
+        <v>5683</v>
+      </c>
+    </row>
+    <row r="676" spans="1:40">
+      <c r="A676" s="1" t="s">
+        <v>5684</v>
+      </c>
+      <c r="B676" s="1" t="s">
+        <v>5685</v>
+      </c>
+      <c r="C676" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D676" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E676" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F676" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G676" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H676" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I676" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J676" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K676" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L676" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="M676" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="N676" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O676" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P676" s="1" t="s">
+        <v>5686</v>
+      </c>
+      <c r="Q676" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="R676" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S676" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T676" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U676" s="1" t="s">
+        <v>5687</v>
+      </c>
+      <c r="V676" s="1" t="s">
+        <v>5688</v>
+      </c>
+      <c r="W676" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X676" s="1" t="s">
+        <v>5689</v>
+      </c>
+      <c r="Y676" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z676" s="1" t="s">
+        <v>5690</v>
+      </c>
+      <c r="AA676" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="AB676" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AC676" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD676" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE676" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF676" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG676" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH676" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI676" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ676" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK676" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL676" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM676" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN676" s="1" t="s">
+        <v>5691</v>
+      </c>
+    </row>
+    <row r="677" spans="1:40">
+      <c r="A677" s="1" t="s">
+        <v>5692</v>
+      </c>
+      <c r="B677" s="1" t="s">
+        <v>5693</v>
+      </c>
+      <c r="C677" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D677" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E677" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K677" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L677" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M677" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N677" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O677" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P677" s="1" t="s">
+        <v>5694</v>
+      </c>
+      <c r="Q677" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="R677" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S677" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T677" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U677" s="1" t="s">
+        <v>5695</v>
+      </c>
+      <c r="V677" s="1" t="s">
+        <v>5696</v>
+      </c>
+      <c r="W677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X677" s="1" t="s">
+        <v>5697</v>
+      </c>
+      <c r="Y677" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z677" s="1" t="s">
+        <v>5698</v>
+      </c>
+      <c r="AA677" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB677" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC677" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD677" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE677" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF677" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG677" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH677" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI677" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ677" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK677" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL677" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM677" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN677" s="1" t="s">
+        <v>5699</v>
+      </c>
+    </row>
+    <row r="678" spans="1:40">
+      <c r="A678" s="1" t="s">
+        <v>5700</v>
+      </c>
+      <c r="B678" s="1" t="s">
+        <v>5701</v>
+      </c>
+      <c r="C678" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D678" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E678" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F678" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H678" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="I678" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="J678" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K678" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L678" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="M678" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N678" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O678" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P678" s="1" t="s">
+        <v>5702</v>
+      </c>
+      <c r="Q678" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R678" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S678" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T678" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U678" s="1" t="s">
+        <v>5703</v>
+      </c>
+      <c r="V678" s="1" t="s">
+        <v>5704</v>
+      </c>
+      <c r="W678" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X678" s="1" t="s">
+        <v>5705</v>
+      </c>
+      <c r="Y678" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z678" s="1" t="s">
+        <v>5706</v>
+      </c>
+      <c r="AA678" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB678" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AC678" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD678" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE678" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF678" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG678" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH678" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI678" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ678" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK678" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL678" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM678" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN678" s="1" t="s">
+        <v>5707</v>
+      </c>
+    </row>
+    <row r="679" spans="1:40">
+      <c r="A679" s="1" t="s">
+        <v>5708</v>
+      </c>
+      <c r="B679" s="1" t="s">
+        <v>5709</v>
+      </c>
+      <c r="C679" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D679" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E679" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F679" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G679" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H679" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I679" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J679" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K679" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L679" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M679" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N679" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O679" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P679" s="1" t="s">
+        <v>5710</v>
+      </c>
+      <c r="Q679" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R679" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S679" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T679" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U679" s="1" t="s">
+        <v>5711</v>
+      </c>
+      <c r="V679" s="1" t="s">
+        <v>5712</v>
+      </c>
+      <c r="W679" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X679" s="1" t="s">
+        <v>5713</v>
+      </c>
+      <c r="Y679" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z679" s="1" t="s">
+        <v>5714</v>
+      </c>
+      <c r="AA679" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB679" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC679" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD679" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE679" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF679" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG679" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH679" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI679" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ679" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK679" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL679" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM679" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN679" s="1" t="s">
+        <v>5715</v>
+      </c>
+    </row>
+    <row r="680" spans="1:40">
+      <c r="A680" s="1" t="s">
+        <v>5716</v>
+      </c>
+      <c r="B680" s="1" t="s">
+        <v>5717</v>
+      </c>
+      <c r="C680" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D680" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E680" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F680" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G680" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H680" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I680" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J680" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K680" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L680" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M680" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N680" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O680" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P680" s="1" t="s">
+        <v>5718</v>
+      </c>
+      <c r="Q680" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R680" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S680" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T680" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U680" s="1" t="s">
+        <v>5719</v>
+      </c>
+      <c r="V680" s="1" t="s">
+        <v>5720</v>
+      </c>
+      <c r="W680" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X680" s="1" t="s">
+        <v>5721</v>
+      </c>
+      <c r="Y680" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z680" s="1" t="s">
+        <v>5722</v>
+      </c>
+      <c r="AA680" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB680" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC680" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD680" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE680" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF680" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG680" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH680" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AI680" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ680" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK680" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL680" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM680" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN680" s="1" t="s">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="681" spans="1:40">
+      <c r="A681" s="1" t="s">
+        <v>5724</v>
+      </c>
+      <c r="B681" s="1" t="s">
+        <v>5725</v>
+      </c>
+      <c r="C681" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D681" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E681" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F681" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G681" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H681" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="I681" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="J681" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K681" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L681" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M681" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N681" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O681" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P681" s="1" t="s">
+        <v>5726</v>
+      </c>
+      <c r="Q681" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R681" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S681" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T681" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U681" s="1" t="s">
+        <v>5727</v>
+      </c>
+      <c r="V681" s="1" t="s">
+        <v>5728</v>
+      </c>
+      <c r="W681" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X681" s="1" t="s">
+        <v>5729</v>
+      </c>
+      <c r="Y681" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z681" s="1" t="s">
+        <v>5730</v>
+      </c>
+      <c r="AA681" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB681" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC681" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD681" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE681" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF681" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG681" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH681" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI681" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ681" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK681" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL681" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM681" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN681" s="1" t="s">
+        <v>5731</v>
+      </c>
+    </row>
+    <row r="682" spans="1:40">
+      <c r="A682" s="1" t="s">
+        <v>5732</v>
+      </c>
+      <c r="B682" s="1" t="s">
+        <v>5733</v>
+      </c>
+      <c r="C682" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D682" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E682" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K682" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L682" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M682" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N682" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O682" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="P682" s="1" t="s">
+        <v>5734</v>
+      </c>
+      <c r="Q682" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R682" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S682" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T682" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U682" s="1" t="s">
+        <v>5735</v>
+      </c>
+      <c r="V682" s="1" t="s">
+        <v>5736</v>
+      </c>
+      <c r="W682" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X682" s="1" t="s">
+        <v>5737</v>
+      </c>
+      <c r="Y682" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z682" s="1" t="s">
+        <v>5738</v>
+      </c>
+      <c r="AA682" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB682" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC682" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD682" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE682" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="AF682" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG682" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="AH682" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="AI682" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK682" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM682" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN682" s="1" t="s">
+        <v>5739</v>
+      </c>
+    </row>
+    <row r="683" spans="1:40">
+      <c r="A683" s="1" t="s">
+        <v>5740</v>
+      </c>
+      <c r="B683" s="1" t="s">
+        <v>5741</v>
+      </c>
+      <c r="C683" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D683" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E683" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F683" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G683" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H683" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I683" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J683" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K683" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L683" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="M683" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N683" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O683" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P683" s="1" t="s">
+        <v>5742</v>
+      </c>
+      <c r="Q683" s="1" t="s">
+        <v>5743</v>
+      </c>
+      <c r="R683" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S683" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T683" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U683" s="1" t="s">
+        <v>5744</v>
+      </c>
+      <c r="V683" s="1" t="s">
+        <v>5745</v>
+      </c>
+      <c r="W683" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X683" s="1" t="s">
+        <v>5746</v>
+      </c>
+      <c r="Y683" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z683" s="1" t="s">
+        <v>5747</v>
+      </c>
+      <c r="AA683" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AB683" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AC683" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD683" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE683" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF683" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG683" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH683" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI683" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ683" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK683" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL683" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM683" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN683" s="1" t="s">
+        <v>5748</v>
+      </c>
+    </row>
+    <row r="684" spans="1:40">
+      <c r="A684" s="1" t="s">
+        <v>5749</v>
+      </c>
+      <c r="B684" s="1" t="s">
+        <v>5750</v>
+      </c>
+      <c r="C684" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D684" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E684" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F684" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G684" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H684" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I684" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J684" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K684" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L684" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M684" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N684" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O684" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P684" s="1" t="s">
+        <v>5751</v>
+      </c>
+      <c r="Q684" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R684" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S684" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T684" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U684" s="1" t="s">
+        <v>5752</v>
+      </c>
+      <c r="V684" s="1" t="s">
+        <v>5753</v>
+      </c>
+      <c r="W684" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X684" s="1" t="s">
+        <v>5754</v>
+      </c>
+      <c r="Y684" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z684" s="1" t="s">
+        <v>5747</v>
+      </c>
+      <c r="AA684" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB684" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC684" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD684" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE684" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF684" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG684" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH684" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI684" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ684" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK684" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL684" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM684" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN684" s="1" t="s">
+        <v>5755</v>
+      </c>
+    </row>
+    <row r="685" spans="1:40">
+      <c r="A685" s="1" t="s">
+        <v>5756</v>
+      </c>
+      <c r="B685" s="1" t="s">
+        <v>5757</v>
+      </c>
+      <c r="C685" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E685" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F685" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G685" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H685" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I685" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J685" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K685" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L685" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M685" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N685" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O685" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P685" s="1" t="s">
+        <v>5758</v>
+      </c>
+      <c r="Q685" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R685" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S685" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T685" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U685" s="1" t="s">
+        <v>5759</v>
+      </c>
+      <c r="V685" s="1" t="s">
+        <v>5760</v>
+      </c>
+      <c r="W685" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X685" s="1" t="s">
+        <v>5761</v>
+      </c>
+      <c r="Y685" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z685" s="1" t="s">
+        <v>5762</v>
+      </c>
+      <c r="AA685" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB685" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC685" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD685" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE685" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF685" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG685" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH685" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI685" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ685" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK685" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL685" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM685" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN685" s="1" t="s">
+        <v>5763</v>
+      </c>
+    </row>
+    <row r="686" spans="1:40">
+      <c r="A686" s="1" t="s">
+        <v>5764</v>
+      </c>
+      <c r="B686" s="1" t="s">
+        <v>5765</v>
+      </c>
+      <c r="C686" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D686" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E686" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F686" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G686" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H686" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I686" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J686" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K686" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L686" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="M686" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="N686" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O686" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P686" s="1" t="s">
+        <v>4696</v>
+      </c>
+      <c r="Q686" s="1" t="s">
+        <v>5591</v>
+      </c>
+      <c r="R686" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S686" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T686" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U686" s="1" t="s">
+        <v>5766</v>
+      </c>
+      <c r="V686" s="1" t="s">
+        <v>5767</v>
+      </c>
+      <c r="W686" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X686" s="1" t="s">
+        <v>5768</v>
+      </c>
+      <c r="Y686" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z686" s="1" t="s">
+        <v>5769</v>
+      </c>
+      <c r="AA686" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB686" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC686" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD686" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE686" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF686" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG686" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH686" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI686" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ686" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK686" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL686" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM686" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN686" s="1" t="s">
+        <v>5770</v>
+      </c>
+    </row>
+    <row r="687" spans="1:40">
+      <c r="A687" s="1" t="s">
+        <v>5771</v>
+      </c>
+      <c r="B687" s="1" t="s">
+        <v>5772</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D687" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E687" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F687" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G687" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H687" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I687" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J687" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K687" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L687" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="M687" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="N687" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O687" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P687" s="1" t="s">
+        <v>5773</v>
+      </c>
+      <c r="Q687" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="R687" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S687" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T687" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U687" s="1" t="s">
+        <v>5774</v>
+      </c>
+      <c r="V687" s="1" t="s">
+        <v>5775</v>
+      </c>
+      <c r="W687" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X687" s="1" t="s">
+        <v>5776</v>
+      </c>
+      <c r="Y687" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z687" s="1" t="s">
+        <v>5777</v>
+      </c>
+      <c r="AA687" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="AB687" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AC687" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD687" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE687" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF687" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG687" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH687" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI687" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ687" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK687" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL687" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM687" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN687" s="1" t="s">
+        <v>5778</v>
+      </c>
+    </row>
+    <row r="688" spans="1:40">
+      <c r="A688" s="1" t="s">
+        <v>5779</v>
+      </c>
+      <c r="B688" s="1" t="s">
+        <v>5780</v>
+      </c>
+      <c r="C688" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E688" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K688" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L688" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M688" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N688" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O688" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P688" s="1" t="s">
+        <v>5781</v>
+      </c>
+      <c r="Q688" s="1" t="s">
+        <v>5782</v>
+      </c>
+      <c r="R688" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="S688" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T688" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U688" s="1" t="s">
+        <v>5783</v>
+      </c>
+      <c r="V688" s="1" t="s">
+        <v>5784</v>
+      </c>
+      <c r="W688" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X688" s="1" t="s">
+        <v>5785</v>
+      </c>
+      <c r="Y688" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z688" s="1" t="s">
+        <v>5786</v>
+      </c>
+      <c r="AA688" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB688" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC688" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD688" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE688" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF688" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG688" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH688" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI688" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ688" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK688" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL688" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM688" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN688" s="1" t="s">
+        <v>5787</v>
+      </c>
+    </row>
+    <row r="689" spans="1:40">
+      <c r="A689" s="1" t="s">
+        <v>5788</v>
+      </c>
+      <c r="B689" s="1" t="s">
+        <v>5789</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E689" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F689" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G689" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H689" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I689" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J689" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K689" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L689" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M689" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N689" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O689" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P689" s="1" t="s">
+        <v>5790</v>
+      </c>
+      <c r="Q689" s="1" t="s">
+        <v>5617</v>
+      </c>
+      <c r="R689" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S689" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T689" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U689" s="1" t="s">
+        <v>5791</v>
+      </c>
+      <c r="V689" s="1" t="s">
+        <v>5792</v>
+      </c>
+      <c r="W689" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X689" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="Y689" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z689" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="AA689" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB689" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC689" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD689" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE689" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF689" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG689" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH689" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI689" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ689" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK689" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL689" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM689" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN689" s="1" t="s">
+        <v>5795</v>
+      </c>
+    </row>
+    <row r="690" spans="1:40">
+      <c r="A690" s="1" t="s">
+        <v>5796</v>
+      </c>
+      <c r="B690" s="1" t="s">
+        <v>5797</v>
+      </c>
+      <c r="C690" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D690" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E690" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F690" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G690" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H690" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I690" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J690" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K690" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L690" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M690" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N690" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O690" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P690" s="1" t="s">
+        <v>5798</v>
+      </c>
+      <c r="Q690" s="1" t="s">
+        <v>5670</v>
+      </c>
+      <c r="R690" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S690" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T690" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U690" s="1" t="s">
+        <v>5799</v>
+      </c>
+      <c r="V690" s="1" t="s">
+        <v>5800</v>
+      </c>
+      <c r="W690" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X690" s="1" t="s">
+        <v>5801</v>
+      </c>
+      <c r="Y690" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z690" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="AA690" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB690" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC690" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD690" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE690" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF690" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG690" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH690" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI690" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ690" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK690" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL690" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM690" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN690" s="1" t="s">
+        <v>5802</v>
+      </c>
+    </row>
+    <row r="691" spans="1:40">
+      <c r="A691" s="1" t="s">
+        <v>5803</v>
+      </c>
+      <c r="B691" s="1" t="s">
+        <v>5804</v>
+      </c>
+      <c r="C691" s="1" t="s">
+        <v>5589</v>
+      </c>
+      <c r="D691" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E691" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F691" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G691" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H691" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I691" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J691" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K691" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L691" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M691" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N691" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O691" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P691" s="1" t="s">
+        <v>5805</v>
+      </c>
+      <c r="Q691" s="1" t="s">
+        <v>5600</v>
+      </c>
+      <c r="R691" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S691" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T691" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U691" s="1" t="s">
+        <v>5806</v>
+      </c>
+      <c r="V691" s="1" t="s">
+        <v>5807</v>
+      </c>
+      <c r="W691" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X691" s="1" t="s">
+        <v>5808</v>
+      </c>
+      <c r="Y691" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z691" s="1" t="s">
+        <v>5794</v>
+      </c>
+      <c r="AA691" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB691" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC691" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD691" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE691" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF691" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG691" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AH691" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AI691" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ691" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK691" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL691" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM691" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN691" s="1" t="s">
+        <v>5809</v>
+      </c>
+    </row>
+    <row r="692" spans="1:40">
+      <c r="A692" s="1" t="s">
+        <v>5810</v>
+      </c>
+      <c r="B692" s="1" t="s">
+        <v>5811</v>
+      </c>
+      <c r="C692" s="1" t="s">
+        <v>5625</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E692" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F692" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G692" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H692" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I692" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J692" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K692" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L692" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M692" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N692" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O692" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P692" s="1" t="s">
+        <v>5812</v>
+      </c>
+      <c r="Q692" s="1" t="s">
+        <v>5231</v>
+      </c>
+      <c r="R692" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="S692" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T692" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U692" s="1" t="s">
+        <v>5813</v>
+      </c>
+      <c r="V692" s="1" t="s">
+        <v>5814</v>
+      </c>
+      <c r="W692" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X692" s="1" t="s">
+        <v>5815</v>
+      </c>
+      <c r="Y692" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z692" s="1" t="s">
+        <v>5816</v>
+      </c>
+      <c r="AA692" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB692" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC692" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD692" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE692" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF692" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG692" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH692" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI692" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ692" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK692" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL692" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM692" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN692" s="1" t="s">
+        <v>5817</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AN662"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aggiornato delivery.xlsx da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/delivery.xlsx
+++ b/delivery.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21325" uniqueCount="2905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22555" uniqueCount="3029">
   <si>
     <t>Codice</t>
   </si>
@@ -8732,6 +8732,378 @@
   </si>
   <si>
     <t>TRECCARICHI GIOVANNI</t>
+  </si>
+  <si>
+    <t>ADSL1004639746</t>
+  </si>
+  <si>
+    <t>91825502</t>
+  </si>
+  <si>
+    <t>19/08/2025</t>
+  </si>
+  <si>
+    <t>CONTRADA STALLONE SNC</t>
+  </si>
+  <si>
+    <t>19/08/2025 10:30</t>
+  </si>
+  <si>
+    <t>DTU0066378285</t>
+  </si>
+  <si>
+    <t>G600070456</t>
+  </si>
+  <si>
+    <t>E70091825502</t>
+  </si>
+  <si>
+    <t>01/08/2025 10:14</t>
+  </si>
+  <si>
+    <t>B37064814</t>
+  </si>
+  <si>
+    <t>ADSL1004641401</t>
+  </si>
+  <si>
+    <t>91836507</t>
+  </si>
+  <si>
+    <t>30 - Sospensione</t>
+  </si>
+  <si>
+    <t>VIA GIOACHINO ROSSINI 66</t>
+  </si>
+  <si>
+    <t>19/08/2025 08:30</t>
+  </si>
+  <si>
+    <t>DTU0066240541</t>
+  </si>
+  <si>
+    <t>93114750130</t>
+  </si>
+  <si>
+    <t>E70091836507</t>
+  </si>
+  <si>
+    <t>B37073218</t>
+  </si>
+  <si>
+    <t>ADSL1004673866</t>
+  </si>
+  <si>
+    <t>92045565</t>
+  </si>
+  <si>
+    <t>VIA CIRO MENOTTI 73</t>
+  </si>
+  <si>
+    <t>DTU0066566297</t>
+  </si>
+  <si>
+    <t>0931587364</t>
+  </si>
+  <si>
+    <t>E70092045565</t>
+  </si>
+  <si>
+    <t>09/08/2025 15:00</t>
+  </si>
+  <si>
+    <t>B37276988</t>
+  </si>
+  <si>
+    <t>ADSL1004677050</t>
+  </si>
+  <si>
+    <t>92065874</t>
+  </si>
+  <si>
+    <t>VIA LUIGI FORNACIARI 2</t>
+  </si>
+  <si>
+    <t>DTU0066529591</t>
+  </si>
+  <si>
+    <t>0931861804</t>
+  </si>
+  <si>
+    <t>E70092065874</t>
+  </si>
+  <si>
+    <t>11/08/2025 12:40</t>
+  </si>
+  <si>
+    <t>B37304293</t>
+  </si>
+  <si>
+    <t>ADSL1004688361</t>
+  </si>
+  <si>
+    <t>92141408</t>
+  </si>
+  <si>
+    <t>VIA MULINO 60</t>
+  </si>
+  <si>
+    <t>DTU0066603811</t>
+  </si>
+  <si>
+    <t>93114741109</t>
+  </si>
+  <si>
+    <t>E70092141408</t>
+  </si>
+  <si>
+    <t>14/08/2025 11:50</t>
+  </si>
+  <si>
+    <t>B37377400</t>
+  </si>
+  <si>
+    <t>ADSL1004605079</t>
+  </si>
+  <si>
+    <t>91598068</t>
+  </si>
+  <si>
+    <t>A PALO/COLONNINA</t>
+  </si>
+  <si>
+    <t>VIA SAN BENEDETTO DA NORCIA 1</t>
+  </si>
+  <si>
+    <t>DTU0066272355</t>
+  </si>
+  <si>
+    <t>0931861517</t>
+  </si>
+  <si>
+    <t>E70091598068</t>
+  </si>
+  <si>
+    <t>24/07/2025 08:00</t>
+  </si>
+  <si>
+    <t>B36854289</t>
+  </si>
+  <si>
+    <t>ADSL1004652056</t>
+  </si>
+  <si>
+    <t>91902786</t>
+  </si>
+  <si>
+    <t>VIA ASSORO 5</t>
+  </si>
+  <si>
+    <t>19/08/2025 13:00</t>
+  </si>
+  <si>
+    <t>DTU0066469100</t>
+  </si>
+  <si>
+    <t>0931317416</t>
+  </si>
+  <si>
+    <t>E70091902786</t>
+  </si>
+  <si>
+    <t>04/08/2025 19:06</t>
+  </si>
+  <si>
+    <t>B37138426</t>
+  </si>
+  <si>
+    <t>ADSL1004686435</t>
+  </si>
+  <si>
+    <t>92128845</t>
+  </si>
+  <si>
+    <t>VIA SALVO RANDONE 14</t>
+  </si>
+  <si>
+    <t>DTU0065658987</t>
+  </si>
+  <si>
+    <t>0931316699</t>
+  </si>
+  <si>
+    <t>E70092128845</t>
+  </si>
+  <si>
+    <t>13/08/2025 16:52</t>
+  </si>
+  <si>
+    <t>B37361698</t>
+  </si>
+  <si>
+    <t>ADSL1004689965</t>
+  </si>
+  <si>
+    <t>92152704</t>
+  </si>
+  <si>
+    <t>VIALE SCALA GRECA 384/C</t>
+  </si>
+  <si>
+    <t>DTU0066619959</t>
+  </si>
+  <si>
+    <t>0931759315</t>
+  </si>
+  <si>
+    <t>E70092152704</t>
+  </si>
+  <si>
+    <t>14/08/2025 17:40</t>
+  </si>
+  <si>
+    <t>B37385921</t>
+  </si>
+  <si>
+    <t>ADSL1004649946</t>
+  </si>
+  <si>
+    <t>91888590</t>
+  </si>
+  <si>
+    <t>VIA SILVIO PELLICO 82</t>
+  </si>
+  <si>
+    <t>DTU0066369715</t>
+  </si>
+  <si>
+    <t>93114758217</t>
+  </si>
+  <si>
+    <t>E70091888590</t>
+  </si>
+  <si>
+    <t>04/08/2025 13:36</t>
+  </si>
+  <si>
+    <t>B37127905</t>
+  </si>
+  <si>
+    <t>ADSL1004653591</t>
+  </si>
+  <si>
+    <t>91912319</t>
+  </si>
+  <si>
+    <t>VIA CRISTOFORO COLOMBO 34</t>
+  </si>
+  <si>
+    <t>DTU0065903949</t>
+  </si>
+  <si>
+    <t>0931967846</t>
+  </si>
+  <si>
+    <t>E70091912319</t>
+  </si>
+  <si>
+    <t>05/08/2025 10:24</t>
+  </si>
+  <si>
+    <t>B37150239</t>
+  </si>
+  <si>
+    <t>ADSL1004661523</t>
+  </si>
+  <si>
+    <t>91968292</t>
+  </si>
+  <si>
+    <t>VIA PALESTRO 192</t>
+  </si>
+  <si>
+    <t>19/08/2025 15:00</t>
+  </si>
+  <si>
+    <t>DTU0066514019</t>
+  </si>
+  <si>
+    <t>0931942405</t>
+  </si>
+  <si>
+    <t>E70091968292</t>
+  </si>
+  <si>
+    <t>B37198425</t>
+  </si>
+  <si>
+    <t>ADSL1004688010</t>
+  </si>
+  <si>
+    <t>92138636</t>
+  </si>
+  <si>
+    <t>VIALE PIETRO NENNI 5</t>
+  </si>
+  <si>
+    <t>DTU0066619160</t>
+  </si>
+  <si>
+    <t>93114739747</t>
+  </si>
+  <si>
+    <t>E70092138636</t>
+  </si>
+  <si>
+    <t>B37375217</t>
+  </si>
+  <si>
+    <t>ADSL1004692461</t>
+  </si>
+  <si>
+    <t>92166651</t>
+  </si>
+  <si>
+    <t>VIA ORAZIO NELSON 33</t>
+  </si>
+  <si>
+    <t>DTU0066646406</t>
+  </si>
+  <si>
+    <t>0931861063</t>
+  </si>
+  <si>
+    <t>E70092166651</t>
+  </si>
+  <si>
+    <t>16/08/2025 13:46</t>
+  </si>
+  <si>
+    <t>B37408081</t>
+  </si>
+  <si>
+    <t>ADSL1004662531</t>
+  </si>
+  <si>
+    <t>91973547</t>
+  </si>
+  <si>
+    <t>VIA GIOVANNI HUSS 100</t>
+  </si>
+  <si>
+    <t>DTU0066518548</t>
+  </si>
+  <si>
+    <t>0931861789</t>
+  </si>
+  <si>
+    <t>E70091973547</t>
+  </si>
+  <si>
+    <t>06/08/2025 19:28</t>
+  </si>
+  <si>
+    <t>B37202498</t>
   </si>
 </sst>
 </file>
@@ -8741,10 +9113,15 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-410]d\-mmm;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8773,12 +9150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -9073,10 +9452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO531"/>
+  <dimension ref="A1:AO561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="E494" sqref="E494"/>
+    <sheetView tabSelected="1" topLeftCell="A526" workbookViewId="0">
+      <selection activeCell="A538" sqref="A538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -74161,6 +74540,3756 @@
         <v>2903</v>
       </c>
     </row>
+    <row r="532" spans="1:41">
+      <c r="A532" s="1" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>2906</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E532" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F532" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G532" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H532" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I532" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J532" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K532" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L532" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M532" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N532" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O532" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P532" s="1" t="s">
+        <v>2908</v>
+      </c>
+      <c r="Q532" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R532" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S532" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T532" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U532" s="1" t="s">
+        <v>2910</v>
+      </c>
+      <c r="V532" s="1" t="s">
+        <v>2911</v>
+      </c>
+      <c r="W532" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X532" s="1" t="s">
+        <v>2912</v>
+      </c>
+      <c r="Y532" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z532" s="1" t="s">
+        <v>2913</v>
+      </c>
+      <c r="AA532" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB532" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC532" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD532" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE532" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF532" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG532" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH532" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI532" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ532" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK532" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL532" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM532" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN532" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AO532" s="1" t="s">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="533" spans="1:41">
+      <c r="A533" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E533" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K533" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L533" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M533" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N533" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O533" s="1" t="s">
+        <v>2917</v>
+      </c>
+      <c r="P533" s="1" t="s">
+        <v>2918</v>
+      </c>
+      <c r="Q533" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R533" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S533" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T533" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U533" s="1" t="s">
+        <v>2920</v>
+      </c>
+      <c r="V533" s="1" t="s">
+        <v>2921</v>
+      </c>
+      <c r="W533" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X533" s="1" t="s">
+        <v>2922</v>
+      </c>
+      <c r="Y533" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z533" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="AA533" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB533" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC533" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD533" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE533" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF533" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG533" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH533" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI533" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK533" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL533" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM533" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN533" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="AO533" s="1" t="s">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="534" spans="1:41">
+      <c r="A534" s="1" t="s">
+        <v>2924</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>2925</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D534" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E534" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F534" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G534" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H534" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I534" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J534" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K534" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L534" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M534" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N534" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O534" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P534" s="1" t="s">
+        <v>2926</v>
+      </c>
+      <c r="Q534" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R534" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S534" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T534" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U534" s="1" t="s">
+        <v>2927</v>
+      </c>
+      <c r="V534" s="1" t="s">
+        <v>2928</v>
+      </c>
+      <c r="W534" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X534" s="1" t="s">
+        <v>2929</v>
+      </c>
+      <c r="Y534" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z534" s="1" t="s">
+        <v>2930</v>
+      </c>
+      <c r="AA534" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB534" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC534" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD534" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE534" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF534" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG534" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH534" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI534" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ534" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK534" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL534" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM534" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN534" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO534" s="1" t="s">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="535" spans="1:41">
+      <c r="A535" s="1" t="s">
+        <v>2932</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>2933</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D535" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E535" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F535" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G535" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H535" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I535" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J535" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K535" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L535" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M535" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N535" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O535" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P535" s="1" t="s">
+        <v>2934</v>
+      </c>
+      <c r="Q535" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R535" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S535" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T535" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U535" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="V535" s="1" t="s">
+        <v>2936</v>
+      </c>
+      <c r="W535" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X535" s="1" t="s">
+        <v>2937</v>
+      </c>
+      <c r="Y535" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z535" s="1" t="s">
+        <v>2938</v>
+      </c>
+      <c r="AA535" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB535" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC535" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD535" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE535" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF535" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG535" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH535" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI535" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ535" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK535" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL535" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM535" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN535" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="AO535" s="1" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="536" spans="1:41">
+      <c r="A536" s="1" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>2941</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E536" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F536" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G536" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H536" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I536" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J536" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K536" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L536" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M536" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N536" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O536" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P536" s="1" t="s">
+        <v>2942</v>
+      </c>
+      <c r="Q536" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R536" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S536" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T536" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U536" s="1" t="s">
+        <v>2943</v>
+      </c>
+      <c r="V536" s="1" t="s">
+        <v>2944</v>
+      </c>
+      <c r="W536" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X536" s="1" t="s">
+        <v>2945</v>
+      </c>
+      <c r="Y536" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z536" s="1" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AA536" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB536" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC536" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD536" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE536" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF536" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG536" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH536" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI536" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ536" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK536" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL536" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM536" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN536" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="AO536" s="1" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="537" spans="1:41">
+      <c r="A537" s="1" t="s">
+        <v>2948</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>2949</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D537" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E537" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F537" s="1" t="s">
+        <v>2462</v>
+      </c>
+      <c r="G537" s="1" t="s">
+        <v>2950</v>
+      </c>
+      <c r="H537" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I537" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J537" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K537" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L537" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M537" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N537" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O537" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P537" s="1" t="s">
+        <v>2951</v>
+      </c>
+      <c r="Q537" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R537" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="S537" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T537" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U537" s="1" t="s">
+        <v>2952</v>
+      </c>
+      <c r="V537" s="1" t="s">
+        <v>2953</v>
+      </c>
+      <c r="W537" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X537" s="1" t="s">
+        <v>2954</v>
+      </c>
+      <c r="Y537" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z537" s="1" t="s">
+        <v>2955</v>
+      </c>
+      <c r="AA537" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB537" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC537" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD537" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE537" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF537" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG537" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH537" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI537" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ537" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK537" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL537" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM537" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN537" s="1" t="s">
+        <v>2523</v>
+      </c>
+      <c r="AO537" s="1" t="s">
+        <v>2956</v>
+      </c>
+    </row>
+    <row r="538" spans="1:41">
+      <c r="A538" s="1" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E538" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F538" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G538" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H538" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I538" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J538" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K538" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L538" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M538" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N538" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O538" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P538" s="1" t="s">
+        <v>2959</v>
+      </c>
+      <c r="Q538" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R538" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="S538" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T538" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U538" s="1" t="s">
+        <v>2961</v>
+      </c>
+      <c r="V538" s="1" t="s">
+        <v>2962</v>
+      </c>
+      <c r="W538" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X538" s="1" t="s">
+        <v>2963</v>
+      </c>
+      <c r="Y538" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z538" s="1" t="s">
+        <v>2964</v>
+      </c>
+      <c r="AA538" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB538" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC538" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD538" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE538" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF538" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG538" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH538" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI538" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ538" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK538" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL538" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM538" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN538" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="AO538" s="1" t="s">
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="539" spans="1:41">
+      <c r="A539" s="1" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>2967</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D539" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E539" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K539" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L539" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M539" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N539" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O539" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P539" s="1" t="s">
+        <v>2968</v>
+      </c>
+      <c r="Q539" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R539" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="S539" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T539" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U539" s="1" t="s">
+        <v>2969</v>
+      </c>
+      <c r="V539" s="1" t="s">
+        <v>2970</v>
+      </c>
+      <c r="W539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X539" s="1" t="s">
+        <v>2971</v>
+      </c>
+      <c r="Y539" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z539" s="1" t="s">
+        <v>2972</v>
+      </c>
+      <c r="AA539" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB539" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC539" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD539" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE539" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF539" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG539" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH539" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI539" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK539" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL539" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM539" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN539" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="AO539" s="1" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="540" spans="1:41">
+      <c r="A540" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E540" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F540" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G540" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H540" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I540" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J540" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K540" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L540" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M540" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N540" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O540" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P540" s="1" t="s">
+        <v>2976</v>
+      </c>
+      <c r="Q540" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R540" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="S540" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T540" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U540" s="1" t="s">
+        <v>2977</v>
+      </c>
+      <c r="V540" s="1" t="s">
+        <v>2978</v>
+      </c>
+      <c r="W540" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X540" s="1" t="s">
+        <v>2979</v>
+      </c>
+      <c r="Y540" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z540" s="1" t="s">
+        <v>2980</v>
+      </c>
+      <c r="AA540" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB540" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC540" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD540" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE540" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF540" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG540" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH540" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI540" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ540" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK540" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL540" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM540" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN540" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO540" s="1" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="541" spans="1:41">
+      <c r="A541" s="1" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>2983</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E541" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F541" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G541" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H541" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I541" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J541" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K541" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L541" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M541" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N541" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O541" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P541" s="1" t="s">
+        <v>2984</v>
+      </c>
+      <c r="Q541" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R541" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="S541" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T541" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U541" s="1" t="s">
+        <v>2985</v>
+      </c>
+      <c r="V541" s="1" t="s">
+        <v>2986</v>
+      </c>
+      <c r="W541" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X541" s="1" t="s">
+        <v>2987</v>
+      </c>
+      <c r="Y541" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z541" s="1" t="s">
+        <v>2988</v>
+      </c>
+      <c r="AA541" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB541" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC541" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD541" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE541" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF541" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG541" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH541" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI541" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ541" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK541" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL541" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM541" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN541" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AO541" s="1" t="s">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="542" spans="1:41">
+      <c r="A542" s="1" t="s">
+        <v>2990</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>2991</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D542" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E542" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F542" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G542" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H542" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I542" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J542" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K542" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L542" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M542" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N542" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O542" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P542" s="1" t="s">
+        <v>2992</v>
+      </c>
+      <c r="Q542" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R542" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="S542" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T542" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U542" s="1" t="s">
+        <v>2993</v>
+      </c>
+      <c r="V542" s="1" t="s">
+        <v>2994</v>
+      </c>
+      <c r="W542" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X542" s="1" t="s">
+        <v>2995</v>
+      </c>
+      <c r="Y542" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z542" s="1" t="s">
+        <v>2996</v>
+      </c>
+      <c r="AA542" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB542" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC542" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD542" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE542" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF542" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG542" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH542" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI542" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ542" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK542" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL542" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM542" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN542" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="AO542" s="1" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="543" spans="1:41">
+      <c r="A543" s="1" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D543" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E543" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F543" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G543" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H543" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I543" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J543" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K543" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L543" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M543" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N543" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O543" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P543" s="1" t="s">
+        <v>3000</v>
+      </c>
+      <c r="Q543" s="1" t="s">
+        <v>3001</v>
+      </c>
+      <c r="R543" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="S543" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T543" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U543" s="1" t="s">
+        <v>3002</v>
+      </c>
+      <c r="V543" s="1" t="s">
+        <v>3003</v>
+      </c>
+      <c r="W543" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X543" s="1" t="s">
+        <v>3004</v>
+      </c>
+      <c r="Y543" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z543" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="AA543" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB543" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC543" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD543" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE543" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF543" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG543" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH543" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI543" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ543" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK543" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL543" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM543" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN543" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO543" s="1" t="s">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="544" spans="1:41">
+      <c r="A544" s="1" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>3007</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D544" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E544" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K544" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L544" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M544" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N544" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O544" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P544" s="1" t="s">
+        <v>3008</v>
+      </c>
+      <c r="Q544" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R544" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="S544" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T544" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U544" s="1" t="s">
+        <v>3009</v>
+      </c>
+      <c r="V544" s="1" t="s">
+        <v>3010</v>
+      </c>
+      <c r="W544" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X544" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="Y544" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z544" s="1" t="s">
+        <v>2465</v>
+      </c>
+      <c r="AA544" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB544" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC544" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD544" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE544" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF544" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG544" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH544" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI544" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ544" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK544" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL544" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM544" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN544" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="AO544" s="1" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="545" spans="1:41">
+      <c r="A545" s="1" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D545" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E545" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F545" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G545" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H545" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I545" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J545" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K545" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L545" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M545" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N545" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O545" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P545" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="Q545" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R545" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="S545" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T545" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U545" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="V545" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="W545" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X545" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="Y545" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z545" s="1" t="s">
+        <v>3019</v>
+      </c>
+      <c r="AA545" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB545" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC545" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD545" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE545" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF545" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG545" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH545" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI545" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ545" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK545" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL545" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM545" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN545" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO545" s="1" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="546" spans="1:41">
+      <c r="A546" s="1" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>3022</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D546" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E546" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K546" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L546" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M546" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N546" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O546" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P546" s="1" t="s">
+        <v>3023</v>
+      </c>
+      <c r="Q546" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R546" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S546" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T546" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U546" s="1" t="s">
+        <v>3024</v>
+      </c>
+      <c r="V546" s="1" t="s">
+        <v>3025</v>
+      </c>
+      <c r="W546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X546" s="1" t="s">
+        <v>3026</v>
+      </c>
+      <c r="Y546" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z546" s="1" t="s">
+        <v>3027</v>
+      </c>
+      <c r="AA546" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB546" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC546" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD546" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE546" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF546" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG546" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH546" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI546" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK546" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL546" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM546" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN546" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="AO546" s="1" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="547" spans="1:41">
+      <c r="A547" s="2" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B547" s="2" t="s">
+        <v>2906</v>
+      </c>
+      <c r="C547" s="2" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D547" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E547" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F547" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G547" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H547" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I547" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J547" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K547" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L547" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M547" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N547" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O547" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P547" s="2" t="s">
+        <v>2908</v>
+      </c>
+      <c r="Q547" s="2" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R547" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S547" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T547" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U547" s="2" t="s">
+        <v>2910</v>
+      </c>
+      <c r="V547" s="2" t="s">
+        <v>2911</v>
+      </c>
+      <c r="W547" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="X547" s="2" t="s">
+        <v>2912</v>
+      </c>
+      <c r="Y547" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z547" s="2" t="s">
+        <v>2913</v>
+      </c>
+      <c r="AA547" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB547" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC547" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD547" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE547" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF547" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG547" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH547" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI547" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ547" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK547" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL547" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM547" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN547" s="2" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AO547" s="2" t="s">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="548" spans="1:41">
+      <c r="A548" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D548" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E548" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K548" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L548" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M548" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N548" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O548" s="1" t="s">
+        <v>2917</v>
+      </c>
+      <c r="P548" s="1" t="s">
+        <v>2918</v>
+      </c>
+      <c r="Q548" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R548" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S548" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T548" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U548" s="1" t="s">
+        <v>2920</v>
+      </c>
+      <c r="V548" s="1" t="s">
+        <v>2921</v>
+      </c>
+      <c r="W548" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X548" s="1" t="s">
+        <v>2922</v>
+      </c>
+      <c r="Y548" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z548" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="AA548" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB548" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC548" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD548" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE548" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF548" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG548" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH548" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI548" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK548" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL548" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM548" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN548" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="AO548" s="1" t="s">
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="549" spans="1:41">
+      <c r="A549" s="1" t="s">
+        <v>2924</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>2925</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D549" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E549" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F549" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G549" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H549" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I549" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J549" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K549" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L549" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M549" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N549" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O549" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P549" s="1" t="s">
+        <v>2926</v>
+      </c>
+      <c r="Q549" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R549" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S549" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T549" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U549" s="1" t="s">
+        <v>2927</v>
+      </c>
+      <c r="V549" s="1" t="s">
+        <v>2928</v>
+      </c>
+      <c r="W549" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X549" s="1" t="s">
+        <v>2929</v>
+      </c>
+      <c r="Y549" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z549" s="1" t="s">
+        <v>2930</v>
+      </c>
+      <c r="AA549" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB549" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC549" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD549" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE549" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF549" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG549" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH549" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI549" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ549" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK549" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL549" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM549" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN549" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO549" s="1" t="s">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="550" spans="1:41">
+      <c r="A550" s="1" t="s">
+        <v>2932</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>2933</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D550" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E550" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F550" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G550" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H550" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I550" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J550" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K550" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L550" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M550" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N550" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O550" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P550" s="1" t="s">
+        <v>2934</v>
+      </c>
+      <c r="Q550" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R550" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S550" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T550" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U550" s="1" t="s">
+        <v>2935</v>
+      </c>
+      <c r="V550" s="1" t="s">
+        <v>2936</v>
+      </c>
+      <c r="W550" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X550" s="1" t="s">
+        <v>2937</v>
+      </c>
+      <c r="Y550" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z550" s="1" t="s">
+        <v>2938</v>
+      </c>
+      <c r="AA550" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB550" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC550" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD550" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE550" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF550" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG550" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH550" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI550" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ550" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK550" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL550" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM550" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN550" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="AO550" s="1" t="s">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="551" spans="1:41">
+      <c r="A551" s="1" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>2941</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D551" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E551" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F551" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G551" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H551" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I551" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J551" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K551" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L551" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M551" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N551" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O551" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P551" s="1" t="s">
+        <v>2942</v>
+      </c>
+      <c r="Q551" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R551" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S551" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T551" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U551" s="1" t="s">
+        <v>2943</v>
+      </c>
+      <c r="V551" s="1" t="s">
+        <v>2944</v>
+      </c>
+      <c r="W551" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X551" s="1" t="s">
+        <v>2945</v>
+      </c>
+      <c r="Y551" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z551" s="1" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AA551" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB551" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC551" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD551" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE551" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF551" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG551" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH551" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI551" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ551" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK551" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL551" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM551" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN551" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="AO551" s="1" t="s">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="552" spans="1:41">
+      <c r="A552" s="6" t="s">
+        <v>2948</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>2949</v>
+      </c>
+      <c r="C552" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D552" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E552" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F552" s="1" t="s">
+        <v>2462</v>
+      </c>
+      <c r="G552" s="1" t="s">
+        <v>2950</v>
+      </c>
+      <c r="H552" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I552" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J552" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K552" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L552" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M552" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N552" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O552" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P552" s="1" t="s">
+        <v>2951</v>
+      </c>
+      <c r="Q552" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R552" s="6" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S552" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T552" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U552" s="1" t="s">
+        <v>2952</v>
+      </c>
+      <c r="V552" s="1" t="s">
+        <v>2953</v>
+      </c>
+      <c r="W552" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X552" s="1" t="s">
+        <v>2954</v>
+      </c>
+      <c r="Y552" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z552" s="1" t="s">
+        <v>2955</v>
+      </c>
+      <c r="AA552" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB552" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC552" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD552" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE552" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF552" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG552" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH552" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI552" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ552" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK552" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL552" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM552" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN552" s="1" t="s">
+        <v>2523</v>
+      </c>
+      <c r="AO552" s="1" t="s">
+        <v>2956</v>
+      </c>
+    </row>
+    <row r="553" spans="1:41">
+      <c r="A553" s="1" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D553" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E553" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F553" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G553" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H553" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I553" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J553" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K553" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L553" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M553" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N553" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O553" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P553" s="1" t="s">
+        <v>2959</v>
+      </c>
+      <c r="Q553" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R553" s="6" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S553" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T553" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U553" s="1" t="s">
+        <v>2961</v>
+      </c>
+      <c r="V553" s="1" t="s">
+        <v>2962</v>
+      </c>
+      <c r="W553" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X553" s="1" t="s">
+        <v>2963</v>
+      </c>
+      <c r="Y553" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z553" s="1" t="s">
+        <v>2964</v>
+      </c>
+      <c r="AA553" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB553" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC553" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD553" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE553" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF553" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG553" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH553" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI553" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ553" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK553" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL553" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM553" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN553" s="1" t="s">
+        <v>2539</v>
+      </c>
+      <c r="AO553" s="1" t="s">
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="554" spans="1:41">
+      <c r="A554" s="1" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>2967</v>
+      </c>
+      <c r="C554" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D554" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E554" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K554" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L554" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M554" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N554" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O554" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P554" s="1" t="s">
+        <v>2968</v>
+      </c>
+      <c r="Q554" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R554" s="6" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S554" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T554" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U554" s="1" t="s">
+        <v>2969</v>
+      </c>
+      <c r="V554" s="1" t="s">
+        <v>2970</v>
+      </c>
+      <c r="W554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X554" s="1" t="s">
+        <v>2971</v>
+      </c>
+      <c r="Y554" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z554" s="1" t="s">
+        <v>2972</v>
+      </c>
+      <c r="AA554" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB554" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC554" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD554" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE554" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF554" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG554" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH554" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI554" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK554" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL554" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM554" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN554" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="AO554" s="1" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="555" spans="1:41">
+      <c r="A555" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="C555" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D555" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E555" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F555" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G555" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H555" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I555" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J555" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K555" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L555" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M555" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N555" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O555" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P555" s="1" t="s">
+        <v>2976</v>
+      </c>
+      <c r="Q555" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R555" s="6" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S555" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T555" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U555" s="1" t="s">
+        <v>2977</v>
+      </c>
+      <c r="V555" s="1" t="s">
+        <v>2978</v>
+      </c>
+      <c r="W555" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X555" s="1" t="s">
+        <v>2979</v>
+      </c>
+      <c r="Y555" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z555" s="1" t="s">
+        <v>2980</v>
+      </c>
+      <c r="AA555" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB555" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC555" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD555" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE555" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF555" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG555" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH555" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI555" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ555" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK555" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL555" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM555" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN555" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO555" s="1" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="556" spans="1:41">
+      <c r="A556" s="1" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>2983</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D556" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E556" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F556" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G556" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H556" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I556" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J556" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K556" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L556" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M556" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N556" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O556" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P556" s="1" t="s">
+        <v>2984</v>
+      </c>
+      <c r="Q556" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R556" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S556" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T556" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U556" s="1" t="s">
+        <v>2985</v>
+      </c>
+      <c r="V556" s="1" t="s">
+        <v>2986</v>
+      </c>
+      <c r="W556" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X556" s="1" t="s">
+        <v>2987</v>
+      </c>
+      <c r="Y556" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z556" s="1" t="s">
+        <v>2988</v>
+      </c>
+      <c r="AA556" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB556" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC556" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD556" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE556" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF556" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG556" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH556" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI556" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ556" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK556" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL556" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM556" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN556" s="1" t="s">
+        <v>2604</v>
+      </c>
+      <c r="AO556" s="1" t="s">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="557" spans="1:41">
+      <c r="A557" s="1" t="s">
+        <v>2990</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>2991</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D557" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E557" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F557" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G557" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H557" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I557" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J557" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K557" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L557" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M557" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N557" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O557" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P557" s="1" t="s">
+        <v>2992</v>
+      </c>
+      <c r="Q557" s="1" t="s">
+        <v>2919</v>
+      </c>
+      <c r="R557" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S557" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T557" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U557" s="1" t="s">
+        <v>2993</v>
+      </c>
+      <c r="V557" s="1" t="s">
+        <v>2994</v>
+      </c>
+      <c r="W557" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X557" s="1" t="s">
+        <v>2995</v>
+      </c>
+      <c r="Y557" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z557" s="1" t="s">
+        <v>2996</v>
+      </c>
+      <c r="AA557" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB557" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC557" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD557" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE557" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF557" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG557" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH557" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI557" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ557" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK557" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL557" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM557" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN557" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="AO557" s="1" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="558" spans="1:41">
+      <c r="A558" s="1" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E558" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F558" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G558" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H558" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I558" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J558" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K558" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L558" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M558" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N558" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O558" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P558" s="1" t="s">
+        <v>3000</v>
+      </c>
+      <c r="Q558" s="1" t="s">
+        <v>3001</v>
+      </c>
+      <c r="R558" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S558" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T558" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U558" s="1" t="s">
+        <v>3002</v>
+      </c>
+      <c r="V558" s="1" t="s">
+        <v>3003</v>
+      </c>
+      <c r="W558" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X558" s="1" t="s">
+        <v>3004</v>
+      </c>
+      <c r="Y558" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z558" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="AA558" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB558" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC558" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD558" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE558" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF558" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG558" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH558" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI558" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ558" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK558" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL558" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM558" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN558" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO558" s="1" t="s">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="559" spans="1:41">
+      <c r="A559" s="1" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>3007</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E559" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K559" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L559" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M559" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N559" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O559" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P559" s="1" t="s">
+        <v>3008</v>
+      </c>
+      <c r="Q559" s="1" t="s">
+        <v>2960</v>
+      </c>
+      <c r="R559" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S559" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T559" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U559" s="1" t="s">
+        <v>3009</v>
+      </c>
+      <c r="V559" s="1" t="s">
+        <v>3010</v>
+      </c>
+      <c r="W559" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X559" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="Y559" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z559" s="1" t="s">
+        <v>2465</v>
+      </c>
+      <c r="AA559" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB559" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC559" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD559" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE559" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF559" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG559" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH559" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI559" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ559" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK559" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL559" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM559" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN559" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="AO559" s="1" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="560" spans="1:41">
+      <c r="A560" s="1" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E560" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F560" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G560" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H560" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I560" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J560" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K560" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L560" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M560" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N560" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O560" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P560" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="Q560" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R560" s="6" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S560" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T560" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U560" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="V560" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="W560" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X560" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="Y560" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z560" s="1" t="s">
+        <v>3019</v>
+      </c>
+      <c r="AA560" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB560" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC560" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD560" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE560" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF560" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG560" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH560" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI560" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ560" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK560" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL560" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM560" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN560" s="1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AO560" s="1" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="561" spans="1:41">
+      <c r="A561" s="1" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>3022</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D561" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E561" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K561" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L561" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M561" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N561" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O561" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P561" s="1" t="s">
+        <v>3023</v>
+      </c>
+      <c r="Q561" s="1" t="s">
+        <v>2909</v>
+      </c>
+      <c r="R561" s="6" t="s">
+        <v>1940</v>
+      </c>
+      <c r="S561" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T561" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U561" s="1" t="s">
+        <v>3024</v>
+      </c>
+      <c r="V561" s="1" t="s">
+        <v>3025</v>
+      </c>
+      <c r="W561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X561" s="1" t="s">
+        <v>3026</v>
+      </c>
+      <c r="Y561" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z561" s="1" t="s">
+        <v>3027</v>
+      </c>
+      <c r="AA561" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB561" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC561" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD561" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE561" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF561" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG561" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH561" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI561" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK561" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL561" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM561" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN561" s="1" t="s">
+        <v>2629</v>
+      </c>
+      <c r="AO561" s="1" t="s">
+        <v>3028</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AN486"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>